<commit_message>
Primera evidencia trabajo en equipo
</commit_message>
<xml_diff>
--- a/CheckLis.xlsx
+++ b/CheckLis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80b25a9b5f40a202/Escritorio/StudyCase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elian\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_F8E06FBC980B768227AB5129936AA0922C5F184C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AE4E24C-5E85-4CD8-874C-D1987B7B743D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D984489-4AAC-47B7-A5FB-AD41FF310492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Intructions" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,6 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mgo1lL5G/eqPuDtBOqeyjwnKq+Vcg=="/>
     </ext>
@@ -40,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="96">
   <si>
     <t>#Tab</t>
   </si>
@@ -373,6 +362,18 @@
   <si>
     <t>Elian y Luis</t>
   </si>
+  <si>
+    <t>Nos reunimos para agregar las primeras actividades en el check list</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evidencia </t>
+  </si>
 </sst>
 </file>
 
@@ -583,7 +584,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -705,12 +706,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -888,6 +904,13 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1511,6 +1534,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>540941</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>52992</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1954609</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1113906</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2217BBF1-2353-40F4-BE94-5B161104E323}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6841332" y="3108930"/>
+          <a:ext cx="1413668" cy="1060914"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -4777,8 +4849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -34178,13 +34250,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B3:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="11.42578125" customWidth="1"/>
+    <col min="1" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="60.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" customWidth="1"/>
+    <col min="6" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" customWidth="1"/>
     <col min="10" max="26" width="11.42578125" customWidth="1"/>
   </cols>
@@ -34210,7 +34285,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18">
         <v>3</v>
       </c>
@@ -34253,6 +34328,26 @@
       <c r="C13" s="56" t="s">
         <v>83</v>
       </c>
+    </row>
+    <row r="15" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="73" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="74">
+        <v>45068</v>
+      </c>
+      <c r="D16" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="73"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -35237,5 +35332,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>